<commit_message>
Modified all routers, seperated endpoint logic, changed post method to put in settings update
</commit_message>
<xml_diff>
--- a/services/backend/xlsx_files/OKmeray's_vocabulary.xlsx
+++ b/services/backend/xlsx_files/OKmeray's_vocabulary.xlsx
@@ -413,7 +413,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:C37"/>
+  <dimension ref="A1:C53"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -441,12 +441,12 @@
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>rebellion</t>
+          <t>minimize</t>
         </is>
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>заколот</t>
+          <t>мінімізувати</t>
         </is>
       </c>
       <c r="C2" t="inlineStr">
@@ -458,131 +458,131 @@
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>loss</t>
+          <t>grand</t>
         </is>
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>втрата</t>
+          <t>грандіозний</t>
         </is>
       </c>
       <c r="C3" t="inlineStr">
         <is>
-          <t>b2</t>
+          <t>c1</t>
         </is>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>consequence</t>
+          <t>undertake</t>
         </is>
       </c>
       <c r="B4" t="inlineStr">
         <is>
-          <t>наслідок</t>
+          <t>здійснювати</t>
         </is>
       </c>
       <c r="C4" t="inlineStr">
         <is>
-          <t>b2</t>
+          <t>c1</t>
         </is>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
-          <t>spread</t>
+          <t>instance</t>
         </is>
       </c>
       <c r="B5" t="inlineStr">
         <is>
-          <t>поширення</t>
+          <t>екземпляр</t>
         </is>
       </c>
       <c r="C5" t="inlineStr">
         <is>
-          <t>b2</t>
+          <t>c1</t>
         </is>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="inlineStr">
         <is>
-          <t>remain</t>
+          <t>insufficient</t>
         </is>
       </c>
       <c r="B6" t="inlineStr">
         <is>
-          <t>залишатися</t>
+          <t>недостатній</t>
         </is>
       </c>
       <c r="C6" t="inlineStr">
         <is>
-          <t>b2</t>
+          <t>c1</t>
         </is>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="inlineStr">
         <is>
-          <t>agreement</t>
+          <t>establishment</t>
         </is>
       </c>
       <c r="B7" t="inlineStr">
         <is>
-          <t>угода</t>
+          <t>створення</t>
         </is>
       </c>
       <c r="C7" t="inlineStr">
         <is>
-          <t>b2</t>
+          <t>c1</t>
         </is>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="inlineStr">
         <is>
-          <t>settle</t>
+          <t>hop</t>
         </is>
       </c>
       <c r="B8" t="inlineStr">
         <is>
-          <t>осідати</t>
+          <t>скакати</t>
         </is>
       </c>
       <c r="C8" t="inlineStr">
         <is>
-          <t>b2</t>
+          <t>c1</t>
         </is>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="inlineStr">
         <is>
-          <t>expansion</t>
+          <t>ally</t>
         </is>
       </c>
       <c r="B9" t="inlineStr">
         <is>
-          <t>розширення</t>
+          <t>союзник</t>
         </is>
       </c>
       <c r="C9" t="inlineStr">
         <is>
-          <t>b2</t>
+          <t>c1</t>
         </is>
       </c>
     </row>
     <row r="10">
       <c r="A10" t="inlineStr">
         <is>
-          <t>empire</t>
+          <t>bronze</t>
         </is>
       </c>
       <c r="B10" t="inlineStr">
         <is>
-          <t>імперія</t>
+          <t>бронза</t>
         </is>
       </c>
       <c r="C10" t="inlineStr">
@@ -594,12 +594,12 @@
     <row r="11">
       <c r="A11" t="inlineStr">
         <is>
-          <t>establishment</t>
+          <t>pose</t>
         </is>
       </c>
       <c r="B11" t="inlineStr">
         <is>
-          <t>створення</t>
+          <t>позу</t>
         </is>
       </c>
       <c r="C11" t="inlineStr">
@@ -611,46 +611,46 @@
     <row r="12">
       <c r="A12" t="inlineStr">
         <is>
-          <t>regional</t>
+          <t>objectively</t>
         </is>
       </c>
       <c r="B12" t="inlineStr">
         <is>
-          <t>регіональний</t>
+          <t>об'єктивно</t>
         </is>
       </c>
       <c r="C12" t="inlineStr">
         <is>
-          <t>b2</t>
+          <t>c1</t>
         </is>
       </c>
     </row>
     <row r="13">
       <c r="A13" t="inlineStr">
         <is>
-          <t>medieval</t>
+          <t>controversy</t>
         </is>
       </c>
       <c r="B13" t="inlineStr">
         <is>
-          <t>середньовічний</t>
+          <t>суперечка</t>
         </is>
       </c>
       <c r="C13" t="inlineStr">
         <is>
-          <t>b2</t>
+          <t>c1</t>
         </is>
       </c>
     </row>
     <row r="14">
       <c r="A14" t="inlineStr">
         <is>
-          <t>bronze</t>
+          <t>reinforce</t>
         </is>
       </c>
       <c r="B14" t="inlineStr">
         <is>
-          <t>бронза</t>
+          <t>підсилювати</t>
         </is>
       </c>
       <c r="C14" t="inlineStr">
@@ -662,131 +662,131 @@
     <row r="15">
       <c r="A15" t="inlineStr">
         <is>
-          <t>portion</t>
+          <t>ample</t>
         </is>
       </c>
       <c r="B15" t="inlineStr">
         <is>
-          <t>порція</t>
+          <t>достатньо</t>
         </is>
       </c>
       <c r="C15" t="inlineStr">
         <is>
-          <t>b2</t>
+          <t>c1</t>
         </is>
       </c>
     </row>
     <row r="16">
       <c r="A16" t="inlineStr">
         <is>
-          <t>state</t>
+          <t>inferior</t>
         </is>
       </c>
       <c r="B16" t="inlineStr">
         <is>
-          <t>держави</t>
+          <t>нижній</t>
         </is>
       </c>
       <c r="C16" t="inlineStr">
         <is>
-          <t>b2</t>
+          <t>c1</t>
         </is>
       </c>
     </row>
     <row r="17">
       <c r="A17" t="inlineStr">
         <is>
-          <t>emerge</t>
+          <t>overestimate</t>
         </is>
       </c>
       <c r="B17" t="inlineStr">
         <is>
-          <t>з’являтися</t>
+          <t>переоцінювати</t>
         </is>
       </c>
       <c r="C17" t="inlineStr">
         <is>
-          <t>b2</t>
+          <t>c1</t>
         </is>
       </c>
     </row>
     <row r="18">
       <c r="A18" t="inlineStr">
         <is>
-          <t>oppose</t>
+          <t>mass</t>
         </is>
       </c>
       <c r="B18" t="inlineStr">
         <is>
-          <t>протидіяти</t>
+          <t>маса</t>
         </is>
       </c>
       <c r="C18" t="inlineStr">
         <is>
-          <t>b2</t>
+          <t>c1</t>
         </is>
       </c>
     </row>
     <row r="19">
       <c r="A19" t="inlineStr">
         <is>
-          <t>nation</t>
+          <t>amateur</t>
         </is>
       </c>
       <c r="B19" t="inlineStr">
         <is>
-          <t>нація</t>
+          <t>аматор</t>
         </is>
       </c>
       <c r="C19" t="inlineStr">
         <is>
-          <t>b2</t>
+          <t>c1</t>
         </is>
       </c>
     </row>
     <row r="20">
       <c r="A20" t="inlineStr">
         <is>
-          <t>strongly</t>
+          <t>obligatory</t>
         </is>
       </c>
       <c r="B20" t="inlineStr">
         <is>
-          <t>сильно</t>
+          <t>обов'язковий</t>
         </is>
       </c>
       <c r="C20" t="inlineStr">
         <is>
-          <t>b2</t>
+          <t>c1</t>
         </is>
       </c>
     </row>
     <row r="21">
       <c r="A21" t="inlineStr">
         <is>
-          <t>middle</t>
+          <t>initiative</t>
         </is>
       </c>
       <c r="B21" t="inlineStr">
         <is>
-          <t>середній</t>
+          <t>ініціатива</t>
         </is>
       </c>
       <c r="C21" t="inlineStr">
         <is>
-          <t>b2</t>
+          <t>c1</t>
         </is>
       </c>
     </row>
     <row r="22">
       <c r="A22" t="inlineStr">
         <is>
-          <t>migration</t>
+          <t>domination</t>
         </is>
       </c>
       <c r="B22" t="inlineStr">
         <is>
-          <t>міграція</t>
+          <t>домінування</t>
         </is>
       </c>
       <c r="C22" t="inlineStr">
@@ -798,29 +798,29 @@
     <row r="23">
       <c r="A23" t="inlineStr">
         <is>
-          <t>external</t>
+          <t>self</t>
         </is>
       </c>
       <c r="B23" t="inlineStr">
         <is>
-          <t>зовнішній</t>
+          <t>я</t>
         </is>
       </c>
       <c r="C23" t="inlineStr">
         <is>
-          <t>b2</t>
+          <t>c1</t>
         </is>
       </c>
     </row>
     <row r="24">
       <c r="A24" t="inlineStr">
         <is>
-          <t>grand</t>
+          <t>toll</t>
         </is>
       </c>
       <c r="B24" t="inlineStr">
         <is>
-          <t>грандіозний</t>
+          <t>плата</t>
         </is>
       </c>
       <c r="C24" t="inlineStr">
@@ -832,63 +832,63 @@
     <row r="25">
       <c r="A25" t="inlineStr">
         <is>
-          <t>legal</t>
+          <t>oneself</t>
         </is>
       </c>
       <c r="B25" t="inlineStr">
         <is>
-          <t>юридичний</t>
+          <t>себе</t>
         </is>
       </c>
       <c r="C25" t="inlineStr">
         <is>
-          <t>b2</t>
+          <t>c1</t>
         </is>
       </c>
     </row>
     <row r="26">
       <c r="A26" t="inlineStr">
         <is>
-          <t>greatly</t>
+          <t>empire</t>
         </is>
       </c>
       <c r="B26" t="inlineStr">
         <is>
-          <t>дуже</t>
+          <t>імперія</t>
         </is>
       </c>
       <c r="C26" t="inlineStr">
         <is>
-          <t>b2</t>
+          <t>c1</t>
         </is>
       </c>
     </row>
     <row r="27">
       <c r="A27" t="inlineStr">
         <is>
-          <t>kingdom</t>
+          <t>weaken</t>
         </is>
       </c>
       <c r="B27" t="inlineStr">
         <is>
-          <t>царство</t>
+          <t>послабити</t>
         </is>
       </c>
       <c r="C27" t="inlineStr">
         <is>
-          <t>b2</t>
+          <t>c1</t>
         </is>
       </c>
     </row>
     <row r="28">
       <c r="A28" t="inlineStr">
         <is>
-          <t>controversy</t>
+          <t>stable</t>
         </is>
       </c>
       <c r="B28" t="inlineStr">
         <is>
-          <t>суперечка</t>
+          <t>конюшня</t>
         </is>
       </c>
       <c r="C28" t="inlineStr">
@@ -900,46 +900,46 @@
     <row r="29">
       <c r="A29" t="inlineStr">
         <is>
-          <t>destruction</t>
+          <t>random</t>
         </is>
       </c>
       <c r="B29" t="inlineStr">
         <is>
-          <t>знищення</t>
+          <t>випадковий</t>
         </is>
       </c>
       <c r="C29" t="inlineStr">
         <is>
-          <t>b2</t>
+          <t>c1</t>
         </is>
       </c>
     </row>
     <row r="30">
       <c r="A30" t="inlineStr">
         <is>
-          <t>latter</t>
+          <t>simplicity</t>
         </is>
       </c>
       <c r="B30" t="inlineStr">
         <is>
-          <t>останній</t>
+          <t>простота</t>
         </is>
       </c>
       <c r="C30" t="inlineStr">
         <is>
-          <t>b2</t>
+          <t>c1</t>
         </is>
       </c>
     </row>
     <row r="31">
       <c r="A31" t="inlineStr">
         <is>
-          <t>ally</t>
+          <t>worthy</t>
         </is>
       </c>
       <c r="B31" t="inlineStr">
         <is>
-          <t>союзник</t>
+          <t>гідний</t>
         </is>
       </c>
       <c r="C31" t="inlineStr">
@@ -951,29 +951,29 @@
     <row r="32">
       <c r="A32" t="inlineStr">
         <is>
-          <t>territory</t>
+          <t>exclude</t>
         </is>
       </c>
       <c r="B32" t="inlineStr">
         <is>
-          <t>територія</t>
+          <t>виключати</t>
         </is>
       </c>
       <c r="C32" t="inlineStr">
         <is>
-          <t>b2</t>
+          <t>c1</t>
         </is>
       </c>
     </row>
     <row r="33">
       <c r="A33" t="inlineStr">
         <is>
-          <t>constitute</t>
+          <t>migration</t>
         </is>
       </c>
       <c r="B33" t="inlineStr">
         <is>
-          <t>складати</t>
+          <t>міграція</t>
         </is>
       </c>
       <c r="C33" t="inlineStr">
@@ -985,29 +985,29 @@
     <row r="34">
       <c r="A34" t="inlineStr">
         <is>
-          <t>major</t>
+          <t>subsequent</t>
         </is>
       </c>
       <c r="B34" t="inlineStr">
         <is>
-          <t>головний</t>
+          <t>наступний</t>
         </is>
       </c>
       <c r="C34" t="inlineStr">
         <is>
-          <t>b2</t>
+          <t>c1</t>
         </is>
       </c>
     </row>
     <row r="35">
       <c r="A35" t="inlineStr">
         <is>
-          <t>weaken</t>
+          <t>rebellion</t>
         </is>
       </c>
       <c r="B35" t="inlineStr">
         <is>
-          <t>послабити</t>
+          <t>заколот</t>
         </is>
       </c>
       <c r="C35" t="inlineStr">
@@ -1019,34 +1019,306 @@
     <row r="36">
       <c r="A36" t="inlineStr">
         <is>
-          <t>establish</t>
+          <t>numerous</t>
         </is>
       </c>
       <c r="B36" t="inlineStr">
         <is>
-          <t>встановлювати</t>
+          <t>численний</t>
         </is>
       </c>
       <c r="C36" t="inlineStr">
         <is>
-          <t>b2</t>
+          <t>c1</t>
         </is>
       </c>
     </row>
     <row r="37">
       <c r="A37" t="inlineStr">
         <is>
-          <t>frost</t>
+          <t>restrict</t>
         </is>
       </c>
       <c r="B37" t="inlineStr">
         <is>
-          <t>мороз</t>
+          <t>обмежувати</t>
         </is>
       </c>
       <c r="C37" t="inlineStr">
         <is>
-          <t>b2</t>
+          <t>c1</t>
+        </is>
+      </c>
+    </row>
+    <row r="38">
+      <c r="A38" t="inlineStr">
+        <is>
+          <t>sufficiently</t>
+        </is>
+      </c>
+      <c r="B38" t="inlineStr">
+        <is>
+          <t>достатньо</t>
+        </is>
+      </c>
+      <c r="C38" t="inlineStr">
+        <is>
+          <t>c1</t>
+        </is>
+      </c>
+    </row>
+    <row r="39">
+      <c r="A39" t="inlineStr">
+        <is>
+          <t>somewhat</t>
+        </is>
+      </c>
+      <c r="B39" t="inlineStr">
+        <is>
+          <t>дещо</t>
+        </is>
+      </c>
+      <c r="C39" t="inlineStr">
+        <is>
+          <t>c1</t>
+        </is>
+      </c>
+    </row>
+    <row r="40">
+      <c r="A40" t="inlineStr">
+        <is>
+          <t>determine</t>
+        </is>
+      </c>
+      <c r="B40" t="inlineStr">
+        <is>
+          <t>визначати</t>
+        </is>
+      </c>
+      <c r="C40" t="inlineStr">
+        <is>
+          <t>c1</t>
+        </is>
+      </c>
+    </row>
+    <row r="41">
+      <c r="A41" t="inlineStr">
+        <is>
+          <t>deficit</t>
+        </is>
+      </c>
+      <c r="B41" t="inlineStr">
+        <is>
+          <t>дефіцит</t>
+        </is>
+      </c>
+      <c r="C41" t="inlineStr">
+        <is>
+          <t>c1</t>
+        </is>
+      </c>
+    </row>
+    <row r="42">
+      <c r="A42" t="inlineStr">
+        <is>
+          <t>engage</t>
+        </is>
+      </c>
+      <c r="B42" t="inlineStr">
+        <is>
+          <t>займатися</t>
+        </is>
+      </c>
+      <c r="C42" t="inlineStr">
+        <is>
+          <t>c1</t>
+        </is>
+      </c>
+    </row>
+    <row r="43">
+      <c r="A43" t="inlineStr">
+        <is>
+          <t>restrain</t>
+        </is>
+      </c>
+      <c r="B43" t="inlineStr">
+        <is>
+          <t>обмежувати</t>
+        </is>
+      </c>
+      <c r="C43" t="inlineStr">
+        <is>
+          <t>c1</t>
+        </is>
+      </c>
+    </row>
+    <row r="44">
+      <c r="A44" t="inlineStr">
+        <is>
+          <t>subsequently</t>
+        </is>
+      </c>
+      <c r="B44" t="inlineStr">
+        <is>
+          <t>згодом</t>
+        </is>
+      </c>
+      <c r="C44" t="inlineStr">
+        <is>
+          <t>c1</t>
+        </is>
+      </c>
+    </row>
+    <row r="45">
+      <c r="A45" t="inlineStr">
+        <is>
+          <t>constitute</t>
+        </is>
+      </c>
+      <c r="B45" t="inlineStr">
+        <is>
+          <t>складати</t>
+        </is>
+      </c>
+      <c r="C45" t="inlineStr">
+        <is>
+          <t>c1</t>
+        </is>
+      </c>
+    </row>
+    <row r="46">
+      <c r="A46" t="inlineStr">
+        <is>
+          <t>sacrifice</t>
+        </is>
+      </c>
+      <c r="B46" t="inlineStr">
+        <is>
+          <t>жертвувати</t>
+        </is>
+      </c>
+      <c r="C46" t="inlineStr">
+        <is>
+          <t>c1</t>
+        </is>
+      </c>
+    </row>
+    <row r="47">
+      <c r="A47" t="inlineStr">
+        <is>
+          <t>purely</t>
+        </is>
+      </c>
+      <c r="B47" t="inlineStr">
+        <is>
+          <t>суто</t>
+        </is>
+      </c>
+      <c r="C47" t="inlineStr">
+        <is>
+          <t>c1</t>
+        </is>
+      </c>
+    </row>
+    <row r="48">
+      <c r="A48" t="inlineStr">
+        <is>
+          <t>technically</t>
+        </is>
+      </c>
+      <c r="B48" t="inlineStr">
+        <is>
+          <t>технічно</t>
+        </is>
+      </c>
+      <c r="C48" t="inlineStr">
+        <is>
+          <t>c1</t>
+        </is>
+      </c>
+    </row>
+    <row r="49">
+      <c r="A49" t="inlineStr">
+        <is>
+          <t>unite</t>
+        </is>
+      </c>
+      <c r="B49" t="inlineStr">
+        <is>
+          <t>об'єднувати</t>
+        </is>
+      </c>
+      <c r="C49" t="inlineStr">
+        <is>
+          <t>c1</t>
+        </is>
+      </c>
+    </row>
+    <row r="50">
+      <c r="A50" t="inlineStr">
+        <is>
+          <t>inclusion</t>
+        </is>
+      </c>
+      <c r="B50" t="inlineStr">
+        <is>
+          <t>включення</t>
+        </is>
+      </c>
+      <c r="C50" t="inlineStr">
+        <is>
+          <t>c1</t>
+        </is>
+      </c>
+    </row>
+    <row r="51">
+      <c r="A51" t="inlineStr">
+        <is>
+          <t>mutual</t>
+        </is>
+      </c>
+      <c r="B51" t="inlineStr">
+        <is>
+          <t>взаємний</t>
+        </is>
+      </c>
+      <c r="C51" t="inlineStr">
+        <is>
+          <t>c1</t>
+        </is>
+      </c>
+    </row>
+    <row r="52">
+      <c r="A52" t="inlineStr">
+        <is>
+          <t>tactic</t>
+        </is>
+      </c>
+      <c r="B52" t="inlineStr">
+        <is>
+          <t>тактика</t>
+        </is>
+      </c>
+      <c r="C52" t="inlineStr">
+        <is>
+          <t>c1</t>
+        </is>
+      </c>
+    </row>
+    <row r="53">
+      <c r="A53" t="inlineStr">
+        <is>
+          <t>seemingly</t>
+        </is>
+      </c>
+      <c r="B53" t="inlineStr">
+        <is>
+          <t>начебто</t>
+        </is>
+      </c>
+      <c r="C53" t="inlineStr">
+        <is>
+          <t>c1</t>
         </is>
       </c>
     </row>

</xml_diff>